<commit_message>
adicionado alguns requisitos no backlog
</commit_message>
<xml_diff>
--- a/Documentação/BackLog-TothLibs.xlsx
+++ b/Documentação/BackLog-TothLibs.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8A1C0E4-AAAE-4707-A4DC-2A75649497DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Documentos\Pasta de clones\grupo05-adsa\Documentação\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F19BED3-6AD2-4BCF-A82A-56F31A84B69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
   <si>
     <t>Estado</t>
   </si>
@@ -52,9 +57,6 @@
     <t>Desejavel</t>
   </si>
   <si>
-    <t>SPRINT</t>
-  </si>
-  <si>
     <t>Planejamento</t>
   </si>
   <si>
@@ -67,9 +69,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>Sprint1</t>
-  </si>
-  <si>
     <t>Cadastro&lt;US1.2&gt;</t>
   </si>
   <si>
@@ -112,9 +111,6 @@
     <t>A aplicação deverá atrelar o livro ao usuario logo após a retirada</t>
   </si>
   <si>
-    <t>O usuario será multado caso exceda o limite de tempo com o livro</t>
-  </si>
-  <si>
     <t>Aplicação&lt;US2.1&gt;</t>
   </si>
   <si>
@@ -127,9 +123,6 @@
     <t>A aplicação deverá rankear os livros mais usados</t>
   </si>
   <si>
-    <t>A aplicação deverá separar livros pro genero e conteúdo</t>
-  </si>
-  <si>
     <t>Aplicação&lt;US4.1&gt;</t>
   </si>
   <si>
@@ -146,13 +139,40 @@
   </si>
   <si>
     <t>{986f3d4e-85bf-45b9-aecd-2ab36224f28d}</t>
+  </si>
+  <si>
+    <t>A aplicação deverá ter um campo de pesquisa para encontrar os livros</t>
+  </si>
+  <si>
+    <t>A aplicação terá o link de compra para os livros</t>
+  </si>
+  <si>
+    <t>A aplicação deverá separar livros por gênero e conteúdo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A aplicação deverá ter uma dashboard com todas as ações do usuário </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A aplicação terá uma resenha do livro, onde o aluno publica algo que ele achou relevante sobre o livro </t>
+  </si>
+  <si>
+    <t>A aplicação deverá ter uma caixa de sugestões</t>
+  </si>
+  <si>
+    <t>O usuário poderá ter contato com o administrador</t>
+  </si>
+  <si>
+    <t>A aplicação deverá disponibilizar um PDF de um e-book</t>
+  </si>
+  <si>
+    <t>A aplicação deverá disponibilizar um PDF do histórico da dashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,13 +188,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <color rgb="FFFF0000"/>
@@ -183,23 +196,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -207,41 +233,113 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
     <dxf>
       <font>
         <sz val="18"/>
       </font>
       <alignment horizontal="center"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -250,6 +348,24 @@
         <color rgb="FFFF0000"/>
       </font>
       <alignment horizontal="center" vertical="center"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -258,6 +374,26 @@
         <color rgb="FFFF0000"/>
       </font>
       <alignment horizontal="center" vertical="center"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -266,12 +402,90 @@
         <color rgb="FFFF0000"/>
       </font>
       <alignment horizontal="center" vertical="center"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <sz val="18"/>
-      </font>
-      <alignment horizontal="center"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -287,12 +501,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC1D4480-120A-4F4E-9F66-6BC644D4E94E}" name="Table2" displayName="Table2" ref="A1:F16" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F16" xr:uid="{FC62B9A2-F0D0-4642-871E-9AAFAAE2A77C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC1D4480-120A-4F4E-9F66-6BC644D4E94E}" name="Table2" displayName="Table2" ref="A1:F22" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F22" xr:uid="{FC62B9A2-F0D0-4642-871E-9AAFAAE2A77C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A63357B8-C26B-43D7-949D-1E0481F48DCF}" name="Estado"/>
-    <tableColumn id="2" xr3:uid="{16F3949E-AC72-4991-97C6-65985CDFFA4B}" name="Funcionalidades"/>
-    <tableColumn id="3" xr3:uid="{82A94399-075C-430D-95D9-B533A2BCE47A}" name="Descrição de requisitos"/>
+    <tableColumn id="1" xr3:uid="{A63357B8-C26B-43D7-949D-1E0481F48DCF}" name="Estado" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{16F3949E-AC72-4991-97C6-65985CDFFA4B}" name="Funcionalidades" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{82A94399-075C-430D-95D9-B533A2BCE47A}" name="Descrição de requisitos" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{CFDE3F53-56C6-486D-A5AE-B147AD101184}" name="Essencial" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{DC6DEEC4-D340-4BD9-B5AF-98F1296BB14C}" name="Importante" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{ECDFAADC-E674-4C8F-9C8D-E7D1CC255F23}" name="Desejavel" dataDxfId="1"/>
@@ -301,18 +515,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3236B910-4233-4C85-9055-37D62520FCBF}" name="Table1" displayName="Table1" ref="G1:G17" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="G1:G17" xr:uid="{F4D37CED-E945-4EEF-BD7B-EEA3F4718609}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{8500A53F-993A-42E0-93CC-6FD371DF7CF1}" name="SPRINT"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -608,16 +812,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
     <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
@@ -625,279 +829,386 @@
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="26.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="26.25">
-      <c r="A3" t="s">
+      <c r="D3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="26.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="30">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="30">
-      <c r="A6" t="s">
+      <c r="C6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" ht="30">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" ht="30">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" ht="30">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" ht="30">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" ht="30">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" ht="30">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" ht="30">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="30">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" ht="30">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" ht="26.25">
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
@@ -909,21 +1220,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>37</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doc: ultimos ajustes no backlog
</commit_message>
<xml_diff>
--- a/Documentação/BackLog-TothLibs.xlsx
+++ b/Documentação/BackLog-TothLibs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanan\Desktop\grupo05-adsa\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas doni\Desktop\Tothlib\grupo05-adsa\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5619C6F-9EC9-4DEE-B79F-28C4CAF83420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE529AE-A1DD-4942-BD93-503074260BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="45">
   <si>
     <t>Estado</t>
   </si>
@@ -96,9 +96,6 @@
     <t xml:space="preserve">A aplicação deve ter a relação de livros Indisponiveis </t>
   </si>
   <si>
-    <t>Aplicação&lt;US???&gt;</t>
-  </si>
-  <si>
     <t>A aplicação deverá atrelar o livro ao usuario logo após a retirada</t>
   </si>
   <si>
@@ -169,6 +166,12 @@
   </si>
   <si>
     <t>Aplicação&lt;SB&gt;</t>
+  </si>
+  <si>
+    <t>Aplicação&lt;US2.4&gt;</t>
+  </si>
+  <si>
+    <t>Aplicação&lt;US1.2&gt;</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -817,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +860,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>7</v>
@@ -889,7 +892,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>11</v>
@@ -905,7 +908,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>12</v>
@@ -921,7 +924,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>14</v>
@@ -969,10 +972,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>8</v>
@@ -985,10 +988,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
@@ -1001,10 +1004,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1020,7 +1023,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
@@ -1033,10 +1036,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1053,10 +1056,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1073,10 +1076,10 @@
         <v>6</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11" t="s">
@@ -1093,10 +1096,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
@@ -1113,10 +1116,10 @@
         <v>6</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
@@ -1129,10 +1132,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="12" t="s">
@@ -1146,10 +1149,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1163,10 +1166,10 @@
         <v>6</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11" t="s">
@@ -1180,10 +1183,10 @@
         <v>6</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
@@ -1197,10 +1200,10 @@
         <v>6</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
@@ -1227,17 +1230,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>